<commit_message>
add plots examples a more experiements
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -7,8 +7,8 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="fraudk" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="p2p" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="credit_card" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="gateway_credit_card" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="pageblocks" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
@@ -528,7 +528,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>fraudk</t>
+          <t>credit_card</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -548,27 +548,27 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>77.82 +- 2.21</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>99.86 +- 0.01</t>
+          <t>78.02 +- 2.25</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>99.87 +- 0.01</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>60.87 +- 0.67</t>
+          <t>60.93 +- 0.68</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>88.15 +- 1.25</t>
+          <t>88.26 +- 1.27</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>88.84 +- 1.11</t>
+          <t>88.94 +- 1.13</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
@@ -840,7 +840,7 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
@@ -1332,7 +1332,7 @@
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D18" s="1" t="n">
@@ -1576,7 +1576,7 @@
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D23" s="1" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D33" s="1" t="n">
@@ -2312,7 +2312,7 @@
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D38" s="1" t="n">
@@ -2894,7 +2894,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>p2p</t>
+          <t>gateway_credit_card</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>51.47 +- 0.15</t>
+          <t>51.53 +- 0.43</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -2924,17 +2924,17 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>67.43 +- 0.15</t>
+          <t>67.26 +- 0.31</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>71.74 +- 0.1</t>
+          <t>71.79 +- 0.3</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>75.74 +- 0.07</t>
+          <t>75.77 +- 0.21</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
@@ -2944,7 +2944,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>1500</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -2962,7 +2962,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>76.48 +- 0.45</t>
+          <t>76.15 +- 0.74</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -2980,17 +2980,17 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>60.47 +- 0.14</t>
+          <t>60.36 +- 0.23</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>87.43 +- 0.26</t>
+          <t>87.24 +- 0.43</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>88.21 +- 0.22</t>
+          <t>88.05 +- 0.37</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -3005,7 +3005,7 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>90.32 +- 1.66</t>
+          <t>89.83 +- 1.67</t>
         </is>
       </c>
     </row>
@@ -3206,7 +3206,7 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
@@ -3698,7 +3698,7 @@
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D18" s="1" t="n">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>64.6 +- 1.48</t>
+          <t>64.47 +- 1.02</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -3716,32 +3716,32 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>56.37 +- 0.56</t>
+          <t>56.32 +- 0.39</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>80.36 +- 0.92</t>
+          <t>80.27 +- 0.63</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>82.28 +- 0.74</t>
+          <t>82.21 +- 0.51</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>0.57 +- 0.01</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>1500</t>
+          <t>0.57 +- 0.0</t>
+        </is>
+      </c>
+      <c r="K18" s="2" t="inlineStr">
+        <is>
+          <t>750</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>86.46 +- 0.25</t>
+          <t>87.24 +- 0.63</t>
         </is>
       </c>
     </row>
@@ -3942,7 +3942,7 @@
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D23" s="1" t="n">
@@ -4434,7 +4434,7 @@
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D33" s="1" t="n">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>65.76 +- 2.37</t>
+          <t>66.29 +- 1.4</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -4452,32 +4452,32 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>56.8 +- 0.89</t>
+          <t>57.0 +- 0.52</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>81.07 +- 1.46</t>
+          <t>81.4 +- 0.86</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>82.86 +- 1.19</t>
+          <t>83.12 +- 0.7</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>0.57 +- 0.01</t>
-        </is>
-      </c>
-      <c r="K33" s="2" t="inlineStr">
-        <is>
-          <t>750</t>
+          <t>0.58 +- 0.01</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>86.96 +- 1.46</t>
+          <t>88.43 +- 0.5</t>
         </is>
       </c>
     </row>
@@ -4678,7 +4678,7 @@
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D38" s="1" t="n">
@@ -5280,27 +5280,27 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>86.9 +- 3.95</t>
+          <t>86.61 +- 3.78</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>90.94 +- 0.75</t>
+          <t>90.91 +- 0.74</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>63.45 +- 1.05</t>
+          <t>63.37 +- 1.01</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>88.87 +- 1.74</t>
+          <t>88.71 +- 1.69</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>88.92 +- 1.69</t>
+          <t>88.76 +- 1.64</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -5328,7 +5328,7 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D3" s="1" t="n">
@@ -5572,7 +5572,7 @@
       <c r="B8" s="1" t="n"/>
       <c r="C8" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D8" s="1" t="n">
@@ -6064,7 +6064,7 @@
       </c>
       <c r="C18" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D18" s="1" t="n">
@@ -6308,7 +6308,7 @@
       <c r="B23" s="1" t="n"/>
       <c r="C23" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D23" s="1" t="n">
@@ -6800,7 +6800,7 @@
       </c>
       <c r="C33" s="1" t="inlineStr">
         <is>
-          <t>drop3-boundaries</t>
+          <t>drop3-drop3-boundaries</t>
         </is>
       </c>
       <c r="D33" s="1" t="n">
@@ -7044,7 +7044,7 @@
       <c r="B38" s="1" t="n"/>
       <c r="C38" s="1" t="inlineStr">
         <is>
-          <t>drop3-one</t>
+          <t>drop3-drop3-one</t>
         </is>
       </c>
       <c r="D38" s="1" t="n">

</xml_diff>